<commit_message>
Need 4a. Update enrollment count, charts.
</commit_message>
<xml_diff>
--- a/assets/Enrollments.xlsx
+++ b/assets/Enrollments.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybakos/Dropbox/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybakos/projects/bsse/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="22780" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,6 +123,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Enrollments AY 2019-24</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -226,7 +251,7 @@
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,11 +555,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2094575840"/>
-        <c:axId val="2094574704"/>
+        <c:axId val="2048682048"/>
+        <c:axId val="2090225520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2094575840"/>
+        <c:axId val="2048682048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094574704"/>
+        <c:crossAx val="2090225520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -585,7 +610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094574704"/>
+        <c:axId val="2090225520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094575840"/>
+        <c:crossAx val="2048682048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1562,7 +1587,7 @@
   <dimension ref="D11:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1601,7 +1626,7 @@
         <v>16</v>
       </c>
       <c r="I12">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.2">

</xml_diff>